<commit_message>
aggiunto nome, cognome . firma dinamica
</commit_message>
<xml_diff>
--- a/Rimborso.xlsx
+++ b/Rimborso.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t xml:space="preserve">Mese di riferimento:</t>
   </si>
@@ -31,15 +31,9 @@
     <t xml:space="preserve">COGNOME</t>
   </si>
   <si>
-    <t xml:space="preserve">Chellini</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOME</t>
   </si>
   <si>
-    <t xml:space="preserve">Cosimo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Modello auto propria utilizzata</t>
   </si>
   <si>
@@ -85,7 +79,7 @@
     <t xml:space="preserve">TOTALE ---&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Cosimo Chellini</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">___________________________________________________________</t>
@@ -420,9 +414,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>821520</xdr:colOff>
+      <xdr:colOff>821160</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -436,7 +430,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9238320" y="343440"/>
-          <a:ext cx="1889640" cy="1311840"/>
+          <a:ext cx="1889280" cy="1311480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -459,7 +453,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="K39" activeCellId="0" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -540,9 +534,7 @@
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -559,11 +551,9 @@
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -597,7 +587,7 @@
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="1"/>
@@ -616,7 +606,7 @@
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
@@ -635,7 +625,7 @@
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1"/>
@@ -673,40 +663,40 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="M11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="N11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="O11" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1289,7 +1279,7 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
@@ -1330,43 +1320,43 @@
     <row r="38" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K39" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L39" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M39" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N39" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O39" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E40" s="20"/>
       <c r="J40" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L40" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M40" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O40" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>